<commit_message>
Agregado nuevos campos de tipo, segmento y aplicacion en la migracion de los productos
</commit_message>
<xml_diff>
--- a/workspace/recursos/src/main/resources/plantillas_excel/productos.xlsx
+++ b/workspace/recursos/src/main/resources/plantillas_excel/productos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE78718C-FBD5-430E-B334-104C96133F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B06B7-4C42-458D-ACA1-700C63609854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">plantilla!$B$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Precio Venta(Sin Iva)</t>
   </si>
@@ -86,10 +85,28 @@
     <t>Costo</t>
   </si>
   <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>EJEMPLO MIGRADO</t>
+    <t>aplicación</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>segmento</t>
+  </si>
+  <si>
+    <t>aplica ok</t>
+  </si>
+  <si>
+    <t>EJEMPLO MIGRADO 1</t>
+  </si>
+  <si>
+    <t>tipo b1</t>
+  </si>
+  <si>
+    <t>segmento b1</t>
+  </si>
+  <si>
+    <t>b1</t>
   </si>
 </sst>
 </file>
@@ -130,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -206,6 +229,7 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +529,10 @@
     <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
@@ -559,13 +584,22 @@
       <c r="Q1" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="R1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3">
         <v>0.5</v>
@@ -608,6 +642,15 @@
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="7"/>
+      <c r="R2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
En la plantilla de migracion de productos agregando un segundo codigo para migrar
</commit_message>
<xml_diff>
--- a/workspace/recursos/src/main/resources/plantillas_excel/productos.xlsx
+++ b/workspace/recursos/src/main/resources/plantillas_excel/productos.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B06B7-4C42-458D-ACA1-700C63609854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A101D17-5ACE-456A-A32D-C37311CEDD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7350" yWindow="4020" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plantilla" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">plantilla!$B$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">plantilla!$C$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Precio Venta(Sin Iva)</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>b1</t>
+  </si>
+  <si>
+    <t>Código2</t>
+  </si>
+  <si>
+    <t>cod02</t>
   </si>
 </sst>
 </file>
@@ -510,145 +516,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>2</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>3</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>4</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>5</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>12</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>0</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="11" t="s">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>